<commit_message>
imitando o codigo da aula
</commit_message>
<xml_diff>
--- a/Dicionario Suicidio.xlsx
+++ b/Dicionario Suicidio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonyarrais/Documents/Universidade Federal Fluminense/Disciplinas/2020_1/GET00186 - Estatistica Aplicada II/6 - Suicidio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a20a830037c9ff3/Documentos/GitHub/Consultoria-Suicidio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDA1E3EE-0079-9D40-914D-3280D029DE0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{FDA1E3EE-0079-9D40-914D-3280D029DE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35E6E4A8-139B-43BF-A710-E5E0DB2EFB90}"/>
   <bookViews>
-    <workbookView xWindow="10720" yWindow="1460" windowWidth="27440" windowHeight="15220" xr2:uid="{E95BC3B4-1B19-F94C-A564-88B24AA3451C}"/>
+    <workbookView minimized="1" xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{E95BC3B4-1B19-F94C-A564-88B24AA3451C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -499,16 +499,16 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -520,7 +520,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -534,7 +534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>1</v>
       </c>
@@ -542,7 +542,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -550,7 +550,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -558,7 +558,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -572,7 +572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>1</v>
       </c>
@@ -580,7 +580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -594,7 +594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>1</v>
       </c>
@@ -602,7 +602,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -616,7 +616,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>2</v>
       </c>
@@ -624,7 +624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -638,12 +638,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>2</v>
+      </c>
       <c r="D13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>3</v>
       </c>
@@ -651,7 +654,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>4</v>
       </c>
@@ -659,7 +662,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>5</v>
       </c>
@@ -667,7 +670,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>6</v>
       </c>
@@ -675,7 +678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -686,7 +689,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>2</v>
       </c>
@@ -694,7 +697,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>3</v>
       </c>
@@ -702,7 +705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>4</v>
       </c>
@@ -710,7 +713,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>5</v>
       </c>
@@ -718,7 +721,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>6</v>
       </c>
@@ -726,7 +729,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -737,7 +740,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>2</v>
       </c>
@@ -745,7 +748,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>3</v>
       </c>
@@ -753,7 +756,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>4</v>
       </c>
@@ -761,7 +764,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>5</v>
       </c>
@@ -769,7 +772,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>6</v>
       </c>

</xml_diff>